<commit_message>
se añade funcionadlidad de agregar al carrito y validar la compra exitosa
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cristian.palacio\IdeaProjects\com.proyecto.test\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\ProyectoPracticaExpress\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD00E11-954E-4B9A-81E4-69210756F606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="usuarios" sheetId="1" r:id="rId1"/>
-    <sheet name="items carrito" sheetId="2" r:id="rId2"/>
+    <sheet name="Shopping car" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,24 +24,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>usuario</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>standard_user</t>
-  </si>
-  <si>
-    <t>secret_sauce</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bike Light</t>
+  </si>
+  <si>
+    <t>Sauce Labs Onesie</t>
+  </si>
+  <si>
+    <t>Luisa</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Marcos</t>
+  </si>
+  <si>
+    <t>sanchez</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Andres</t>
+  </si>
+  <si>
+    <t>Velez</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Avaible</t>
+  </si>
+  <si>
+    <t>Used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -354,47 +397,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>50012</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>50367</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>50013</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>50154</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>50367</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3D8502-D249-4B87-8413-77A5B4649C79}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se agrega carpeta y funcionalida de screenshot para mirar las imagenes generadas en el modo headless
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\ProyectoPracticaExpress\src\test\resources\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Item Name</t>
   </si>
@@ -87,6 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,116 +402,116 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E6" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.33203125"/>
+    <col min="2" max="2" customWidth="true" width="13.109375"/>
+    <col min="3" max="3" customWidth="true" width="13.0"/>
+    <col min="4" max="4" customWidth="true" width="15.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>50012</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>50367</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>50013</v>
       </c>
-      <c r="E4" t="s">
-        <v>18</v>
+      <c r="E4" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>50154</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>50367</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>17</v>
       </c>
     </row>

</xml_diff>